<commit_message>
Remove hard-coded FYs in COP21 OPU Tool
This aligns with updates to packPSNUxIM, but will break processing for OPU tools out in the wild. Needs further revision.
</commit_message>
<xml_diff>
--- a/inst/extdata/COP21_OPU_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP21_OPU_Data_Pack_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DECC6AA5-C327-0B45-ABDC-5B1665E3A98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F523F21-6120-6741-9EED-871FE1EC8C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10480" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
@@ -159,15 +159,6 @@
     <t>Deduplicated Total</t>
   </si>
   <si>
-    <t>Deduplicated DSD Rollup (FY22)</t>
-  </si>
-  <si>
-    <t>Total Deduplicated Rollup (FY22)</t>
-  </si>
-  <si>
-    <t>Deduplicated TA Rollup (FY22)</t>
-  </si>
-  <si>
     <t>SNU x IM Target Allocation Percentages</t>
   </si>
   <si>
@@ -189,26 +180,8 @@
     <t>MAX - Crosswalk Total</t>
   </si>
   <si>
-    <t>DSD Dedupe Resolution (FY22)</t>
-  </si>
-  <si>
     <t>Confirm or reallocate DataPackTarget values among Mechanisms in row 14.
 Make sure targets have been 100% distributed by confirming Rollup and DataPackTarget columns are equal.</t>
-  </si>
-  <si>
-    <t>Custom DSD Dedupe Allocation (FY22) (% of DataPackTarget)</t>
-  </si>
-  <si>
-    <t>Custom Crosswalk Dedupe Allocation (FY22) (% of DataPackTarget)</t>
-  </si>
-  <si>
-    <t>Crosswalk Dedupe Resolution (FY22)</t>
-  </si>
-  <si>
-    <t>TA Dedupe Resolution (FY22)</t>
-  </si>
-  <si>
-    <t>Custom TA Dedupe Allocation (FY22) (% of DataPackTarget)</t>
   </si>
   <si>
     <t>If "CUSTOM", enter negative Dedupe allocation (%) below, to add to positive IM allocations (%).</t>
@@ -224,6 +197,33 @@
   </si>
   <si>
     <t>COP21 OPU Data Pack</t>
+  </si>
+  <si>
+    <t>Crosswalk Dedupe Resolution</t>
+  </si>
+  <si>
+    <t>Custom Crosswalk Dedupe Allocation (% of DataPackTarget)</t>
+  </si>
+  <si>
+    <t>Total Deduplicated Rollup</t>
+  </si>
+  <si>
+    <t>Deduplicated DSD Rollup</t>
+  </si>
+  <si>
+    <t>Custom DSD Dedupe Allocation (% of DataPackTarget)</t>
+  </si>
+  <si>
+    <t>DSD Dedupe Resolution</t>
+  </si>
+  <si>
+    <t>TA Dedupe Resolution</t>
+  </si>
+  <si>
+    <t>Custom TA Dedupe Allocation (% of DataPackTarget)</t>
+  </si>
+  <si>
+    <t>Deduplicated TA Rollup</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="10" spans="2:2" ht="97" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="82" x14ac:dyDescent="0.9">
@@ -1174,10 +1174,10 @@
   <dimension ref="A1:FS23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="14" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="14" topLeftCell="CB15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="CW15" sqref="CW15"/>
+      <selection pane="bottomRight" activeCell="CV15" sqref="CV15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="H2" s="81"/>
       <c r="I2" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="3" spans="1:175" ht="118" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="89" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" s="90"/>
       <c r="C3" s="7"/>
@@ -1670,30 +1670,30 @@
       <c r="CF3" s="18"/>
       <c r="CG3" s="18"/>
       <c r="CH3" s="57" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="CI3" s="58" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="CJ3" s="70"/>
       <c r="CK3" s="18"/>
       <c r="CL3" s="18"/>
       <c r="CM3" s="18"/>
       <c r="CN3" s="57" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="CO3" s="59" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="CP3" s="70"/>
       <c r="CQ3" s="18"/>
       <c r="CR3" s="18"/>
       <c r="CS3" s="18"/>
       <c r="CT3" s="57" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="CU3" s="58" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="CV3" s="70"/>
       <c r="CW3" s="19"/>
@@ -6795,55 +6795,55 @@
       <c r="CD14" s="55"/>
       <c r="CE14" s="88"/>
       <c r="CF14" s="31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="CG14" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="CH14" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="CI14" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="CJ14" s="73" t="s">
+        <v>47</v>
+      </c>
+      <c r="CK14" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="CL14" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="CM14" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="CH14" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="CI14" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="CJ14" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="CK14" s="31" t="s">
+      <c r="CN14" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="CO14" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="CP14" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="CQ14" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="CR14" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="CL14" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="CM14" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="CN14" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="CO14" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="CP14" s="73" t="s">
-        <v>32</v>
-      </c>
-      <c r="CQ14" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="CR14" s="31" t="s">
-        <v>39</v>
-      </c>
       <c r="CS14" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="CT14" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="CU14" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="CT14" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="CU14" s="25" t="s">
-        <v>48</v>
-      </c>
       <c r="CV14" s="73" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="CW14" s="27" t="str">
         <f t="shared" ref="CW14:EB14" si="0">IF(I14="","",I$14)</f>

</xml_diff>